<commit_message>
Cap column width at 255
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/AdjustToContents.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/AdjustToContents.xlsx
@@ -11,6 +11,7 @@
     <x:sheet name="Adjust Widths 2" sheetId="4" r:id="rId4"/>
     <x:sheet name="Adjust Heights" sheetId="5" r:id="rId5"/>
     <x:sheet name="Adjust Heights 2" sheetId="6" r:id="rId6"/>
+    <x:sheet name="Absurdly wide column" sheetId="7" r:id="rId7"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <x:si>
     <x:t>Tall Row</x:t>
   </x:si>
@@ -2937,6 +2938,12 @@
       </x:rPr>
       <x:t>Hello</x:t>
     </x:r>
+  </x:si>
+  <x:si>
+    <x:t>Some string</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. It has survived not only five centuries, but also the leap into electronic typesetting, remaining essentially unchanged. It was popularised in the 1960s with the release of Letraset sheets containing Lorem Ipsum passages, and more recently with desktop publishing software like Aldus PageMaker including versions of Lorem Ipsum.</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -3980,4 +3987,36 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:B1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="11.920625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="255" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:2">
+      <x:c r="A1" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>